<commit_message>
terminando o app do opera facil
</commit_message>
<xml_diff>
--- a/Prestador/neotin/resultado/relatorio_neotin_APENAS_VALORES.xlsx
+++ b/Prestador/neotin/resultado/relatorio_neotin_APENAS_VALORES.xlsx
@@ -815,7 +815,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -1005,7 +1005,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>

</xml_diff>